<commit_message>
dictionnaire de donne finale et mes test
</commit_message>
<xml_diff>
--- a/dictionnaire de données sgbd.xlsx
+++ b/dictionnaire de données sgbd.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christophe\Desktop\projetapex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christophe\Desktop\projet sgbd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="300">
   <si>
     <t>Nom de l'attribut</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Role</t>
-  </si>
-  <si>
     <t>Cell_Contact</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
   </si>
   <si>
     <t>ID_Equipes</t>
-  </si>
-  <si>
-    <t>Type</t>
   </si>
   <si>
     <t>Ecoles, Gyms, Equipes</t>
@@ -204,13 +198,7 @@
     <t>Nom_Poste</t>
   </si>
   <si>
-    <t>Entree</t>
-  </si>
-  <si>
     <t>Facture</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
   <si>
     <t>Filename</t>
@@ -380,15 +368,6 @@
 Recompenses_Entraineurs</t>
   </si>
   <si>
-    <t>comptes_Utilisateurs</t>
-  </si>
-  <si>
-    <t>ID_Compte</t>
-  </si>
-  <si>
-    <t>Nom_Compte</t>
-  </si>
-  <si>
     <t>Mot_Passe</t>
   </si>
   <si>
@@ -470,9 +449,6 @@
     <t>nom de l'équipe</t>
   </si>
   <si>
-    <t>type de l'équipe</t>
-  </si>
-  <si>
     <t>Identifiant de l'entraineur</t>
   </si>
   <si>
@@ -608,9 +584,6 @@
     <t>date où l'équipement a été retourné</t>
   </si>
   <si>
-    <t>saison de l'inscription</t>
-  </si>
-  <si>
     <t>identifiant du recipiendaire</t>
   </si>
   <si>
@@ -734,12 +707,6 @@
     <t>Date_Transaction</t>
   </si>
   <si>
-    <t>Transaction, Equipes_Tournois,Inscriptions</t>
-  </si>
-  <si>
-    <t>Facture, Transactions</t>
-  </si>
-  <si>
     <t>Photocopie</t>
   </si>
   <si>
@@ -795,6 +762,171 @@
   </si>
   <si>
     <t>9L9L9L</t>
+  </si>
+  <si>
+    <t>Role_contact</t>
+  </si>
+  <si>
+    <t>date_pratique</t>
+  </si>
+  <si>
+    <t>date de la pratique</t>
+  </si>
+  <si>
+    <t>Type_equipe</t>
+  </si>
+  <si>
+    <t>type de l'équipe(Masculin, feminin, mixte)</t>
+  </si>
+  <si>
+    <t>montant_inscription</t>
+  </si>
+  <si>
+    <t>montant nécessaire à l'inscription à l'équipe</t>
+  </si>
+  <si>
+    <t>entraineurs</t>
+  </si>
+  <si>
+    <t>code postal de l'entraineur</t>
+  </si>
+  <si>
+    <t>L9L9L9</t>
+  </si>
+  <si>
+    <t>ID_Equipes_Entraineurs</t>
+  </si>
+  <si>
+    <t>identifiant de equipes_entraineurs</t>
+  </si>
+  <si>
+    <t>Depense</t>
+  </si>
+  <si>
+    <t>Date_facture</t>
+  </si>
+  <si>
+    <t>Transaction, Equipes_Tournois,Inscriptions,Factures</t>
+  </si>
+  <si>
+    <t>quantite</t>
+  </si>
+  <si>
+    <t>shorts</t>
+  </si>
+  <si>
+    <t>quantité de short totale</t>
+  </si>
+  <si>
+    <t>ID_pret</t>
+  </si>
+  <si>
+    <t>ientifiant du prêt d'équipement</t>
+  </si>
+  <si>
+    <t>Inscriptions, récipiendaires</t>
+  </si>
+  <si>
+    <t>sexe</t>
+  </si>
+  <si>
+    <t>joueurs</t>
+  </si>
+  <si>
+    <t>sexe du joueur</t>
+  </si>
+  <si>
+    <t>annee</t>
+  </si>
+  <si>
+    <t>indique l'année du reçu d'impôt</t>
+  </si>
+  <si>
+    <t>Date_Recompense</t>
+  </si>
+  <si>
+    <t>Utilisateurs</t>
+  </si>
+  <si>
+    <t>Nom_Utilisateur</t>
+  </si>
+  <si>
+    <t>ID_Utilisateur</t>
+  </si>
+  <si>
+    <t>ID_Equipes_Tournoi</t>
+  </si>
+  <si>
+    <t>Equipes_Tournoi</t>
+  </si>
+  <si>
+    <t>identifiant equpies_tournoi</t>
+  </si>
+  <si>
+    <t>APEX_ACCESS_CONTROL</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ADMIN_USERNAME</t>
+  </si>
+  <si>
+    <t>ADMIN_PRIVILEGES</t>
+  </si>
+  <si>
+    <t>SETUP_ID</t>
+  </si>
+  <si>
+    <t>CREATED_BY</t>
+  </si>
+  <si>
+    <t>CREATED_ON</t>
+  </si>
+  <si>
+    <t>UPDATED_ON</t>
+  </si>
+  <si>
+    <t>UPDATED_BY</t>
+  </si>
+  <si>
+    <t>identifiant de la table APEX_ACCESS_CONTROL</t>
+  </si>
+  <si>
+    <t>privilèges de l'utilisateur</t>
+  </si>
+  <si>
+    <t>nom de l'utilisateur</t>
+  </si>
+  <si>
+    <t>Identifie le créateur de l'accès</t>
+  </si>
+  <si>
+    <t>date de créaion de l'accès</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifie la dernière personne qui a modifer l'accès </t>
+  </si>
+  <si>
+    <t>date de la dernière modification</t>
+  </si>
+  <si>
+    <t>APEX_ACCESS_SETUP</t>
+  </si>
+  <si>
+    <t>APPLICATION_MODE</t>
+  </si>
+  <si>
+    <t>APPLICATION_ID</t>
+  </si>
+  <si>
+    <t>identifiant de l'application où l'accès est appliqué</t>
+  </si>
+  <si>
+    <t>mode d'accès de l'utilisateur</t>
+  </si>
+  <si>
+    <t>identifaint de APEX_ACCESS_SETUP</t>
   </si>
 </sst>
 </file>
@@ -1000,9 +1132,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1011,6 +1140,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1325,11 +1457,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1360,32 +1490,32 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8"/>
+      <c r="A2" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="8"/>
+      <c r="A3" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -1395,7 +1525,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1403,13 +1533,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>129</v>
+        <v>144</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -1417,89 +1547,83 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>255</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D7" s="7">
-        <v>9999999999</v>
-      </c>
+        <v>215</v>
+      </c>
+      <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>269</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>131</v>
+        <v>270</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="7">
-        <v>9999999999</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
+      <c r="A9" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="8"/>
+      <c r="A10" s="10" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>298</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>136</v>
+        <v>194</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
@@ -1507,13 +1631,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>133</v>
+        <v>198</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
@@ -1521,13 +1645,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>132</v>
+        <v>199</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1535,13 +1659,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -1549,13 +1673,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -1563,83 +1687,91 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D16" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>254</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>27</v>
+        <v>252</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D17" s="7"/>
+        <v>253</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>254</v>
+      </c>
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D18" s="7"/>
+        <v>192</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>244</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>27</v>
+        <v>107</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>217</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>244</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>49</v>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>145</v>
+        <v>229</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1647,69 +1779,69 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>7</v>
+        <v>71</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>30</v>
+      <c r="A23" s="10" t="s">
+        <v>117</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>28</v>
+        <v>114</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>147</v>
+        <v>242</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="15"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="8"/>
+      <c r="A25" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>291</v>
+      </c>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>99</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>36</v>
+        <v>96</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>150</v>
+        <v>206</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1717,10 +1849,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>155</v>
@@ -1731,13 +1863,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>35</v>
+        <v>258</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1745,29 +1877,27 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="D29" s="7">
-        <v>9999999999</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
@@ -1775,13 +1905,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C31" s="7" t="s">
-        <v>153</v>
+        <v>193</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -1789,13 +1919,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>37</v>
+        <v>246</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -1803,13 +1933,13 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
@@ -1817,27 +1947,27 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>38</v>
+      <c r="A35" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>233</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>139</v>
+        <v>236</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
@@ -1845,13 +1975,13 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
@@ -1859,13 +1989,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>42</v>
+        <v>225</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -1873,27 +2003,27 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>43</v>
+      <c r="A39" s="10" t="s">
+        <v>257</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -1901,13 +2031,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
@@ -1915,13 +2045,13 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>163</v>
+        <v>218</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
@@ -1929,13 +2059,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
@@ -1943,13 +2073,13 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
@@ -1957,13 +2087,13 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>235</v>
+        <v>21</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
@@ -1971,13 +2101,13 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
@@ -1985,13 +2115,13 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>233</v>
+        <v>24</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>168</v>
+        <v>131</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
@@ -1999,27 +2129,27 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>234</v>
+        <v>24</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="10" t="s">
-        <v>53</v>
+      <c r="A48" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
@@ -2027,52 +2157,52 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
       <c r="F49" s="8"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
-      <c r="F50" s="8"/>
+      <c r="A50" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="15"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>173</v>
-      </c>
-      <c r="D51" s="7"/>
-      <c r="E51" s="7"/>
-      <c r="F51" s="8"/>
+      <c r="A51" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>294</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>299</v>
+      </c>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="15"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>59</v>
+      <c r="A52" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>174</v>
@@ -2083,13 +2213,13 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>236</v>
+        <v>39</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
@@ -2097,13 +2227,13 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
@@ -2111,13 +2241,13 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>237</v>
+        <v>18</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>60</v>
+        <v>22</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>177</v>
+        <v>125</v>
       </c>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
@@ -2125,41 +2255,41 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>178</v>
+        <v>119</v>
       </c>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="8"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>60</v>
+        <v>30</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>179</v>
+        <v>140</v>
       </c>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
       <c r="F57" s="8"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>66</v>
+    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
@@ -2167,41 +2297,41 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>67</v>
+        <v>255</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>181</v>
+        <v>256</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="8"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D60" s="7"/>
-      <c r="E60" s="7"/>
-      <c r="F60" s="8"/>
+      <c r="A60" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="B60" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="15"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
@@ -2209,13 +2339,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>184</v>
+        <v>129</v>
       </c>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
@@ -2223,38 +2353,38 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>68</v>
+        <v>265</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="8"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="3" t="s">
-        <v>75</v>
+      <c r="A64" s="10" t="s">
+        <v>115</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>186</v>
+        <v>240</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="8"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>68</v>
+        <v>227</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>104</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>187</v>
@@ -2265,13 +2395,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="C66" s="7" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -2279,13 +2409,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
@@ -2293,13 +2423,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>71</v>
+        <v>97</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
@@ -2307,41 +2437,41 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="C69" s="7" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="8"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>81</v>
+      <c r="A70" s="10" t="s">
+        <v>222</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="8"/>
+        <v>108</v>
+      </c>
+      <c r="C70" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="15"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
@@ -2349,13 +2479,13 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>193</v>
+        <v>133</v>
       </c>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
@@ -2363,13 +2493,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>83</v>
+        <v>263</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C73" s="7" t="s">
-        <v>194</v>
+        <v>264</v>
       </c>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
@@ -2377,27 +2507,27 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="8"/>
     </row>
-    <row r="75" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>108</v>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B75" s="11" t="s">
+        <v>233</v>
       </c>
       <c r="C75" s="7" t="s">
-        <v>196</v>
+        <v>234</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
@@ -2405,13 +2535,13 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C76" s="7" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
@@ -2419,13 +2549,13 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C77" s="7" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
@@ -2433,57 +2563,55 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="C78" s="7" t="s">
-        <v>199</v>
+        <v>153</v>
       </c>
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="8"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>86</v>
+        <v>49</v>
+      </c>
+      <c r="B79" s="9" t="s">
+        <v>259</v>
       </c>
       <c r="C79" s="7" t="s">
-        <v>200</v>
+        <v>158</v>
       </c>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="8"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>86</v>
+      <c r="A80" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="D80" s="7" t="s">
-        <v>255</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="8"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C81" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
@@ -2491,13 +2619,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>89</v>
+        <v>19</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>203</v>
+        <v>130</v>
       </c>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
@@ -2505,13 +2633,13 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>86</v>
+        <v>26</v>
       </c>
       <c r="C83" s="7" t="s">
-        <v>204</v>
+        <v>134</v>
       </c>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
@@ -2519,13 +2647,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>205</v>
+        <v>149</v>
       </c>
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
@@ -2533,13 +2661,13 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C85" s="7" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
@@ -2547,13 +2675,13 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>93</v>
+        <v>52</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
@@ -2561,13 +2689,13 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>86</v>
+        <v>48</v>
       </c>
       <c r="C87" s="7" t="s">
-        <v>208</v>
+        <v>159</v>
       </c>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
@@ -2575,27 +2703,27 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="F88" s="8"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B89" s="7" t="s">
-        <v>96</v>
+      <c r="A89" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B89" s="11" t="s">
+        <v>233</v>
       </c>
       <c r="C89" s="7" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
@@ -2603,13 +2731,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
-        <v>97</v>
+        <v>250</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>96</v>
+        <v>27</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>211</v>
+        <v>251</v>
       </c>
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
@@ -2617,27 +2745,27 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>212</v>
+        <v>157</v>
       </c>
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
       <c r="F91" s="8"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>100</v>
+      <c r="A92" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
@@ -2645,13 +2773,13 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>214</v>
+        <v>146</v>
       </c>
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
@@ -2659,13 +2787,13 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
@@ -2673,13 +2801,13 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>216</v>
+        <v>175</v>
       </c>
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
@@ -2687,13 +2815,13 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>217</v>
+        <v>120</v>
       </c>
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
@@ -2701,13 +2829,13 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>114</v>
+        <v>17</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>218</v>
+        <v>126</v>
       </c>
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
@@ -2715,33 +2843,29 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>228</v>
+        <v>7</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>111</v>
+        <v>27</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D98" s="7">
-        <v>9999999999</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D98" s="7"/>
       <c r="E98" s="7"/>
       <c r="F98" s="8"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>229</v>
+        <v>7</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>111</v>
+        <v>34</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="D99" s="7">
-        <v>9999999999</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="8"/>
     </row>
@@ -2750,10 +2874,10 @@
         <v>7</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>111</v>
+        <v>39</v>
       </c>
       <c r="C100" s="7" t="s">
-        <v>221</v>
+        <v>152</v>
       </c>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
@@ -2761,13 +2885,13 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>33</v>
+        <v>83</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>111</v>
+        <v>82</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
@@ -2775,13 +2899,13 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C102" s="7" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
@@ -2789,13 +2913,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C103" s="7" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
@@ -2803,13 +2927,13 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="C104" s="7" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
@@ -2817,29 +2941,27 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="C105" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="D105" s="7" t="s">
-        <v>255</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="D105" s="7"/>
       <c r="E105" s="7"/>
       <c r="F105" s="8"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>110</v>
+        <v>56</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>111</v>
+        <v>53</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>227</v>
+        <v>165</v>
       </c>
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
@@ -2847,27 +2969,27 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>112</v>
+        <v>48</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>239</v>
+        <v>160</v>
       </c>
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
       <c r="F107" s="8"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B108" s="7" t="s">
-        <v>112</v>
+      <c r="A108" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
@@ -2875,27 +2997,27 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="s">
-        <v>231</v>
+        <v>116</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C109" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="D109" s="15"/>
-      <c r="E109" s="15"/>
-      <c r="F109" s="16"/>
+        <v>114</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="D109" s="7"/>
+      <c r="E109" s="7"/>
+      <c r="F109" s="8"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="3" t="s">
-        <v>115</v>
+      <c r="A110" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>113</v>
+        <v>48</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>241</v>
+        <v>162</v>
       </c>
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
@@ -2903,83 +3025,83 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="C111" s="7" t="s">
-        <v>242</v>
+        <v>169</v>
       </c>
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
       <c r="F111" s="8"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="B112" s="11" t="s">
-        <v>244</v>
+      <c r="A112" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>245</v>
+        <v>203</v>
       </c>
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
       <c r="F112" s="8"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B113" s="11" t="s">
-        <v>244</v>
+      <c r="A113" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C113" s="7" t="s">
-        <v>246</v>
+        <v>142</v>
       </c>
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
       <c r="F113" s="8"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B114" s="11" t="s">
-        <v>244</v>
+      <c r="A114" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>247</v>
+        <v>189</v>
       </c>
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
       <c r="F114" s="8"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="10" t="s">
-        <v>118</v>
-      </c>
-      <c r="B115" s="11" t="s">
-        <v>117</v>
+      <c r="A115" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="C115" s="7" t="s">
-        <v>248</v>
+        <v>213</v>
       </c>
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
       <c r="F115" s="8"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B116" s="11" t="s">
-        <v>117</v>
+      <c r="A116" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>261</v>
       </c>
       <c r="C116" s="7" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
@@ -2987,75 +3109,338 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="C117" s="7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
       <c r="F117" s="8"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="10" t="s">
-        <v>122</v>
+      <c r="A118" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>251</v>
-      </c>
-      <c r="D118" s="7"/>
+        <v>137</v>
+      </c>
+      <c r="D118" s="7">
+        <v>9999999999</v>
+      </c>
       <c r="E118" s="7"/>
       <c r="F118" s="8"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="10" t="s">
-        <v>123</v>
+      <c r="A119" s="3" t="s">
+        <v>221</v>
       </c>
       <c r="B119" s="7" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C119" s="7" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
       <c r="F119" s="8"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="10" t="s">
-        <v>124</v>
+      <c r="A120" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>253</v>
+        <v>173</v>
       </c>
       <c r="D120" s="7"/>
       <c r="E120" s="7"/>
       <c r="F120" s="8"/>
     </row>
-    <row r="121" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B121" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C121" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="D121" s="13"/>
-      <c r="E121" s="13"/>
-      <c r="F121" s="14"/>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C121" s="14"/>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="15"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B122" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D122" s="7"/>
+      <c r="E122" s="7"/>
+      <c r="F122" s="8"/>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="8"/>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="8"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="8"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D126" s="7">
+        <v>9999999999</v>
+      </c>
+      <c r="E126" s="7"/>
+      <c r="F126" s="8"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D127" s="7">
+        <v>9999999999</v>
+      </c>
+      <c r="E127" s="7"/>
+      <c r="F127" s="8"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D128" s="7">
+        <v>9999999999</v>
+      </c>
+      <c r="E128" s="7"/>
+      <c r="F128" s="8"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D129" s="7">
+        <v>9999999999</v>
+      </c>
+      <c r="E129" s="7"/>
+      <c r="F129" s="8"/>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="D130" s="7"/>
+      <c r="E130" s="7"/>
+      <c r="F130" s="8"/>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D131" s="7"/>
+      <c r="E131" s="7"/>
+      <c r="F131" s="8"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="D132" s="7"/>
+      <c r="E132" s="7"/>
+      <c r="F132" s="8"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="B133" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C133" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="D133" s="14"/>
+      <c r="E133" s="14"/>
+      <c r="F133" s="15"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="B134" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="C134" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="D134" s="14"/>
+      <c r="E134" s="14"/>
+      <c r="F134" s="15"/>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D135" s="7"/>
+      <c r="E135" s="7"/>
+      <c r="F135" s="8"/>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C136" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D136" s="7"/>
+      <c r="E136" s="7"/>
+      <c r="F136" s="8"/>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C137" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="8"/>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C138" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="D138" s="7"/>
+      <c r="E138" s="7"/>
+      <c r="F138" s="8"/>
+    </row>
+    <row r="139" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B139" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C139" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="D139" s="12"/>
+      <c r="E139" s="12"/>
+      <c r="F139" s="13"/>
     </row>
   </sheetData>
+  <sortState ref="A2:F139">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>